<commit_message>
Fix endpoint (AddOn , Package , Apartment, Booking )
</commit_message>
<xml_diff>
--- a/Documentation/SampleUnitTest.xlsx
+++ b/Documentation/SampleUnitTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\OdaDataService\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_z\OdaWebApi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="3" r:id="rId1"/>
@@ -1798,9 +1798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2176,7 +2174,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,7 +2479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2798,7 +2796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
elka01:add payment model and booking
</commit_message>
<xml_diff>
--- a/Documentation/SampleUnitTest.xlsx
+++ b/Documentation/SampleUnitTest.xlsx
@@ -9,26 +9,29 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Developer" sheetId="14" r:id="rId1"/>
-    <sheet name="Project" sheetId="3" r:id="rId2"/>
-    <sheet name="Plan" sheetId="4" r:id="rId3"/>
-    <sheet name="PlanDetails" sheetId="16" r:id="rId4"/>
-    <sheet name="Automation" sheetId="15" r:id="rId5"/>
-    <sheet name="AutomationDetails" sheetId="17" r:id="rId6"/>
-    <sheet name="AddOns " sheetId="1" r:id="rId7"/>
-    <sheet name="AddonsPerRequest" sheetId="18" r:id="rId8"/>
-    <sheet name="Apartment" sheetId="2" r:id="rId9"/>
-    <sheet name="ApartmentAddons" sheetId="5" r:id="rId10"/>
-    <sheet name="PaymentMethod" sheetId="13" r:id="rId11"/>
-    <sheet name="Booking" sheetId="7" r:id="rId12"/>
-    <sheet name="Customer" sheetId="8" r:id="rId13"/>
-    <sheet name="Invoices" sheetId="9" r:id="rId14"/>
-    <sheet name="User" sheetId="10" r:id="rId15"/>
-    <sheet name="Role" sheetId="11" r:id="rId16"/>
-    <sheet name="Permission" sheetId="12" r:id="rId17"/>
+    <sheet name="PaymentPlan " sheetId="19" r:id="rId2"/>
+    <sheet name="installmentBreakDown" sheetId="21" r:id="rId3"/>
+    <sheet name="ApartmentPayment" sheetId="20" r:id="rId4"/>
+    <sheet name="Project" sheetId="3" r:id="rId5"/>
+    <sheet name="Plan" sheetId="4" r:id="rId6"/>
+    <sheet name="PlanDetails" sheetId="16" r:id="rId7"/>
+    <sheet name="Automation" sheetId="15" r:id="rId8"/>
+    <sheet name="AutomationDetails" sheetId="17" r:id="rId9"/>
+    <sheet name="AddOns " sheetId="1" r:id="rId10"/>
+    <sheet name="AddonsPerRequest" sheetId="18" r:id="rId11"/>
+    <sheet name="Apartment" sheetId="2" r:id="rId12"/>
+    <sheet name="ApartmentAddons" sheetId="5" r:id="rId13"/>
+    <sheet name="PaymentMethod" sheetId="13" r:id="rId14"/>
+    <sheet name="Booking" sheetId="7" r:id="rId15"/>
+    <sheet name="Customer" sheetId="8" r:id="rId16"/>
+    <sheet name="Invoices" sheetId="9" r:id="rId17"/>
+    <sheet name="User" sheetId="10" r:id="rId18"/>
+    <sheet name="Role" sheetId="11" r:id="rId19"/>
+    <sheet name="Permission" sheetId="12" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="182">
   <si>
     <t>AddOns</t>
   </si>
@@ -535,6 +538,57 @@
   </si>
   <si>
     <t>Orascom</t>
+  </si>
+  <si>
+    <t>PaymentPlanId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PaymentPlanName </t>
+  </si>
+  <si>
+    <t>PaymentPlanIcon</t>
+  </si>
+  <si>
+    <t>DownPayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DownPaymentPercentage </t>
+  </si>
+  <si>
+    <t>AdminFees</t>
+  </si>
+  <si>
+    <t>AdminFeesPercentage</t>
+  </si>
+  <si>
+    <t>InterestRate</t>
+  </si>
+  <si>
+    <t>Oda</t>
+  </si>
+  <si>
+    <t>SEVEN</t>
+  </si>
+  <si>
+    <t>NumberOfInstallmentMonths</t>
+  </si>
+  <si>
+    <t>Valu</t>
+  </si>
+  <si>
+    <t>InterestRatePerYearPercentage</t>
+  </si>
+  <si>
+    <t>AmountEachMonth</t>
+  </si>
+  <si>
+    <t>BreakDownId</t>
+  </si>
+  <si>
+    <t>InstallmentMont</t>
+  </si>
+  <si>
+    <t>InstallmentPercentage</t>
   </si>
 </sst>
 </file>
@@ -579,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,6 +646,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -876,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -932,6 +989,486 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>6000</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>4500</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <v>7500</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1">
+        <v>65</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1">
+        <v>72</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="1">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1">
+        <v>110</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1">
+        <v>120</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="1">
+        <v>115</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1">
+        <v>140</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1">
+        <v>155</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="1">
+        <v>136</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -974,7 +1511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1017,13 +1554,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1162,7 +1697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -1334,7 +1869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -1537,7 +2072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -1654,7 +2189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1733,7 +2268,356 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="7">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>60</v>
+      </c>
+      <c r="G2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="7">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>40</v>
+      </c>
+      <c r="G3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="7">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>4</v>
+      </c>
+      <c r="I5" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="7">
+        <v>18</v>
+      </c>
+      <c r="E6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>10</v>
+      </c>
+      <c r="I6" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="7">
+        <v>24</v>
+      </c>
+      <c r="E7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="7">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="7">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>4</v>
+      </c>
+      <c r="I9" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="7">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <v>10</v>
+      </c>
+      <c r="I10" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="7">
+        <v>24</v>
+      </c>
+      <c r="E11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <v>15</v>
+      </c>
+      <c r="I11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="7">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="7">
+        <v>48</v>
+      </c>
+      <c r="E13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="7">
+        <v>60</v>
+      </c>
+      <c r="E14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -2111,7 +2995,1106 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49">
+        <v>11</v>
+      </c>
+      <c r="D49">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>12</v>
+      </c>
+      <c r="D50">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="D63">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>8</v>
+      </c>
+      <c r="D64">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>9</v>
+      </c>
+      <c r="D65">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>11</v>
+      </c>
+      <c r="D67">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>12</v>
+      </c>
+      <c r="D68">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>9</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>9</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>9</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>9</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>9</v>
+      </c>
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="D74">
+        <v>5.56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -2208,7 +4191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2282,7 +4265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -2373,7 +4356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2426,7 +4409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2467,486 +4450,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
-        <v>3000</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1">
-        <v>2500</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1">
-        <v>6000</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <v>4500</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
-        <v>7500</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1">
-        <v>5000</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1">
-        <v>2500</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1">
-        <v>65</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="1">
-        <v>72</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1">
-        <v>84</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="1">
-        <v>110</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="1">
-        <v>120</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="1">
-        <v>115</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1">
-        <v>140</v>
-      </c>
-      <c r="H8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="1">
-        <v>155</v>
-      </c>
-      <c r="H9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="1">
-        <v>136</v>
-      </c>
-      <c r="H10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
elka01:update excel sheet of unit test
</commit_message>
<xml_diff>
--- a/Documentation/SampleUnitTest.xlsx
+++ b/Documentation/SampleUnitTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\OdaWebApi\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\OdaWebApi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Developer" sheetId="14" r:id="rId1"/>
@@ -2997,10 +2997,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:XFD116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4045,6 +4045,2526 @@
       </c>
       <c r="D74">
         <v>5.56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>9</v>
+      </c>
+      <c r="C75">
+        <v>7</v>
+      </c>
+      <c r="D75">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>9</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>9</v>
+      </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>9</v>
+      </c>
+      <c r="C79">
+        <v>11</v>
+      </c>
+      <c r="D79">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>9</v>
+      </c>
+      <c r="C80">
+        <v>12</v>
+      </c>
+      <c r="D80">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>9</v>
+      </c>
+      <c r="C81">
+        <v>13</v>
+      </c>
+      <c r="D81">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>14</v>
+      </c>
+      <c r="D82">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>15</v>
+      </c>
+      <c r="D83">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <v>16</v>
+      </c>
+      <c r="D84">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>9</v>
+      </c>
+      <c r="C85">
+        <v>17</v>
+      </c>
+      <c r="D85">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>9</v>
+      </c>
+      <c r="C86">
+        <v>18</v>
+      </c>
+      <c r="D86">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>10</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="D90">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
+      </c>
+      <c r="D91">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>10</v>
+      </c>
+      <c r="C92">
+        <v>6</v>
+      </c>
+      <c r="D92">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>7</v>
+      </c>
+      <c r="D93">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>10</v>
+      </c>
+      <c r="C94">
+        <v>8</v>
+      </c>
+      <c r="D94">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>9</v>
+      </c>
+      <c r="D95">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>10</v>
+      </c>
+      <c r="D96">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>10</v>
+      </c>
+      <c r="C97">
+        <v>11</v>
+      </c>
+      <c r="D97">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>12</v>
+      </c>
+      <c r="D98">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>10</v>
+      </c>
+      <c r="C99">
+        <v>13</v>
+      </c>
+      <c r="D99">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>14</v>
+      </c>
+      <c r="D100">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>15</v>
+      </c>
+      <c r="D101">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>10</v>
+      </c>
+      <c r="C102">
+        <v>16</v>
+      </c>
+      <c r="D102">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>10</v>
+      </c>
+      <c r="C103">
+        <v>17</v>
+      </c>
+      <c r="D103">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>18</v>
+      </c>
+      <c r="D104">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>19</v>
+      </c>
+      <c r="D105">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>20</v>
+      </c>
+      <c r="D106">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>21</v>
+      </c>
+      <c r="D107">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>22</v>
+      </c>
+      <c r="D108">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>10</v>
+      </c>
+      <c r="C109">
+        <v>23</v>
+      </c>
+      <c r="D109">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>10</v>
+      </c>
+      <c r="C110">
+        <v>24</v>
+      </c>
+      <c r="D110">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>11</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>11</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>11</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+      <c r="D113">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>11</v>
+      </c>
+      <c r="C114">
+        <v>4</v>
+      </c>
+      <c r="D114">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>11</v>
+      </c>
+      <c r="C115">
+        <v>5</v>
+      </c>
+      <c r="D115">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2220</v>
+      </c>
+      <c r="B116">
+        <v>11</v>
+      </c>
+      <c r="C116">
+        <v>6</v>
+      </c>
+      <c r="D116">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>11</v>
+      </c>
+      <c r="C117">
+        <v>7</v>
+      </c>
+      <c r="D117">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>11</v>
+      </c>
+      <c r="C118">
+        <v>8</v>
+      </c>
+      <c r="D118">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>11</v>
+      </c>
+      <c r="C119">
+        <v>9</v>
+      </c>
+      <c r="D119">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>11</v>
+      </c>
+      <c r="C120">
+        <v>10</v>
+      </c>
+      <c r="D120">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>11</v>
+      </c>
+      <c r="C121">
+        <v>11</v>
+      </c>
+      <c r="D121">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>11</v>
+      </c>
+      <c r="C122">
+        <v>12</v>
+      </c>
+      <c r="D122">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>11</v>
+      </c>
+      <c r="C123">
+        <v>13</v>
+      </c>
+      <c r="D123">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>11</v>
+      </c>
+      <c r="C124">
+        <v>14</v>
+      </c>
+      <c r="D124">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>11</v>
+      </c>
+      <c r="C125">
+        <v>15</v>
+      </c>
+      <c r="D125">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>11</v>
+      </c>
+      <c r="C126">
+        <v>16</v>
+      </c>
+      <c r="D126">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>11</v>
+      </c>
+      <c r="C127">
+        <v>17</v>
+      </c>
+      <c r="D127">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>11</v>
+      </c>
+      <c r="C128">
+        <v>18</v>
+      </c>
+      <c r="D128">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>11</v>
+      </c>
+      <c r="C129">
+        <v>19</v>
+      </c>
+      <c r="D129">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>11</v>
+      </c>
+      <c r="C130">
+        <v>20</v>
+      </c>
+      <c r="D130">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>11</v>
+      </c>
+      <c r="C131">
+        <v>21</v>
+      </c>
+      <c r="D131">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>11</v>
+      </c>
+      <c r="C132">
+        <v>22</v>
+      </c>
+      <c r="D132">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>11</v>
+      </c>
+      <c r="C133">
+        <v>23</v>
+      </c>
+      <c r="D133">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>11</v>
+      </c>
+      <c r="C134">
+        <v>24</v>
+      </c>
+      <c r="D134">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>11</v>
+      </c>
+      <c r="C135">
+        <v>25</v>
+      </c>
+      <c r="D135">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>11</v>
+      </c>
+      <c r="C136">
+        <v>26</v>
+      </c>
+      <c r="D136">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>11</v>
+      </c>
+      <c r="C137">
+        <v>27</v>
+      </c>
+      <c r="D137">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>11</v>
+      </c>
+      <c r="C138">
+        <v>28</v>
+      </c>
+      <c r="D138">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>11</v>
+      </c>
+      <c r="C139">
+        <v>29</v>
+      </c>
+      <c r="D139">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>11</v>
+      </c>
+      <c r="C140">
+        <v>30</v>
+      </c>
+      <c r="D140">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>11</v>
+      </c>
+      <c r="C141">
+        <v>31</v>
+      </c>
+      <c r="D141">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>11</v>
+      </c>
+      <c r="C142">
+        <v>32</v>
+      </c>
+      <c r="D142">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>11</v>
+      </c>
+      <c r="C143">
+        <v>33</v>
+      </c>
+      <c r="D143">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>11</v>
+      </c>
+      <c r="C144">
+        <v>34</v>
+      </c>
+      <c r="D144">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>11</v>
+      </c>
+      <c r="C145">
+        <v>35</v>
+      </c>
+      <c r="D145">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>11</v>
+      </c>
+      <c r="C146">
+        <v>36</v>
+      </c>
+      <c r="D146">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>12</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>12</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+      <c r="D148">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>12</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+      <c r="D149">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>12</v>
+      </c>
+      <c r="C150">
+        <v>4</v>
+      </c>
+      <c r="D150">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>12</v>
+      </c>
+      <c r="C151">
+        <v>5</v>
+      </c>
+      <c r="D151">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152">
+        <v>12</v>
+      </c>
+      <c r="C152">
+        <v>6</v>
+      </c>
+      <c r="D152">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153">
+        <v>12</v>
+      </c>
+      <c r="C153">
+        <v>7</v>
+      </c>
+      <c r="D153">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154">
+        <v>12</v>
+      </c>
+      <c r="C154">
+        <v>8</v>
+      </c>
+      <c r="D154">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155">
+        <v>12</v>
+      </c>
+      <c r="C155">
+        <v>9</v>
+      </c>
+      <c r="D155">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156">
+        <v>12</v>
+      </c>
+      <c r="C156">
+        <v>10</v>
+      </c>
+      <c r="D156">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157">
+        <v>12</v>
+      </c>
+      <c r="C157">
+        <v>11</v>
+      </c>
+      <c r="D157">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158">
+        <v>12</v>
+      </c>
+      <c r="C158">
+        <v>12</v>
+      </c>
+      <c r="D158">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159">
+        <v>12</v>
+      </c>
+      <c r="C159">
+        <v>13</v>
+      </c>
+      <c r="D159">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160">
+        <v>12</v>
+      </c>
+      <c r="C160">
+        <v>14</v>
+      </c>
+      <c r="D160">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>12</v>
+      </c>
+      <c r="C161">
+        <v>15</v>
+      </c>
+      <c r="D161">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>12</v>
+      </c>
+      <c r="C162">
+        <v>16</v>
+      </c>
+      <c r="D162">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163">
+        <v>12</v>
+      </c>
+      <c r="C163">
+        <v>17</v>
+      </c>
+      <c r="D163">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164">
+        <v>12</v>
+      </c>
+      <c r="C164">
+        <v>18</v>
+      </c>
+      <c r="D164">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165">
+        <v>12</v>
+      </c>
+      <c r="C165">
+        <v>19</v>
+      </c>
+      <c r="D165">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166">
+        <v>12</v>
+      </c>
+      <c r="C166">
+        <v>20</v>
+      </c>
+      <c r="D166">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167">
+        <v>12</v>
+      </c>
+      <c r="C167">
+        <v>21</v>
+      </c>
+      <c r="D167">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>12</v>
+      </c>
+      <c r="C168">
+        <v>22</v>
+      </c>
+      <c r="D168">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169">
+        <v>12</v>
+      </c>
+      <c r="C169">
+        <v>23</v>
+      </c>
+      <c r="D169">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>12</v>
+      </c>
+      <c r="C170">
+        <v>24</v>
+      </c>
+      <c r="D170">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>12</v>
+      </c>
+      <c r="C171">
+        <v>25</v>
+      </c>
+      <c r="D171">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>12</v>
+      </c>
+      <c r="C172">
+        <v>26</v>
+      </c>
+      <c r="D172">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173">
+        <v>12</v>
+      </c>
+      <c r="C173">
+        <v>27</v>
+      </c>
+      <c r="D173">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174">
+        <v>12</v>
+      </c>
+      <c r="C174">
+        <v>28</v>
+      </c>
+      <c r="D174">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175">
+        <v>12</v>
+      </c>
+      <c r="C175">
+        <v>29</v>
+      </c>
+      <c r="D175">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>12</v>
+      </c>
+      <c r="C176">
+        <v>30</v>
+      </c>
+      <c r="D176">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177">
+        <v>12</v>
+      </c>
+      <c r="C177">
+        <v>31</v>
+      </c>
+      <c r="D177">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178">
+        <v>12</v>
+      </c>
+      <c r="C178">
+        <v>32</v>
+      </c>
+      <c r="D178">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179">
+        <v>12</v>
+      </c>
+      <c r="C179">
+        <v>33</v>
+      </c>
+      <c r="D179">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180">
+        <v>12</v>
+      </c>
+      <c r="C180">
+        <v>34</v>
+      </c>
+      <c r="D180">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181">
+        <v>12</v>
+      </c>
+      <c r="C181">
+        <v>35</v>
+      </c>
+      <c r="D181">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182">
+        <v>12</v>
+      </c>
+      <c r="C182">
+        <v>36</v>
+      </c>
+      <c r="D182">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183">
+        <v>12</v>
+      </c>
+      <c r="C183">
+        <v>37</v>
+      </c>
+      <c r="D183">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184">
+        <v>12</v>
+      </c>
+      <c r="C184">
+        <v>38</v>
+      </c>
+      <c r="D184">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185">
+        <v>12</v>
+      </c>
+      <c r="C185">
+        <v>39</v>
+      </c>
+      <c r="D185">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186">
+        <v>12</v>
+      </c>
+      <c r="C186">
+        <v>40</v>
+      </c>
+      <c r="D186">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187">
+        <v>12</v>
+      </c>
+      <c r="C187">
+        <v>41</v>
+      </c>
+      <c r="D187">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188">
+        <v>12</v>
+      </c>
+      <c r="C188">
+        <v>42</v>
+      </c>
+      <c r="D188">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189">
+        <v>12</v>
+      </c>
+      <c r="C189">
+        <v>43</v>
+      </c>
+      <c r="D189">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190">
+        <v>12</v>
+      </c>
+      <c r="C190">
+        <v>44</v>
+      </c>
+      <c r="D190">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191">
+        <v>12</v>
+      </c>
+      <c r="C191">
+        <v>45</v>
+      </c>
+      <c r="D191">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192">
+        <v>12</v>
+      </c>
+      <c r="C192">
+        <v>46</v>
+      </c>
+      <c r="D192">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193">
+        <v>12</v>
+      </c>
+      <c r="C193">
+        <v>47</v>
+      </c>
+      <c r="D193">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194">
+        <v>12</v>
+      </c>
+      <c r="C194">
+        <v>48</v>
+      </c>
+      <c r="D194">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195">
+        <v>13</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196">
+        <v>13</v>
+      </c>
+      <c r="C196">
+        <v>2</v>
+      </c>
+      <c r="D196">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197">
+        <v>13</v>
+      </c>
+      <c r="C197">
+        <v>3</v>
+      </c>
+      <c r="D197">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198">
+        <v>13</v>
+      </c>
+      <c r="C198">
+        <v>4</v>
+      </c>
+      <c r="D198">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199">
+        <v>13</v>
+      </c>
+      <c r="C199">
+        <v>5</v>
+      </c>
+      <c r="D199">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200">
+        <v>13</v>
+      </c>
+      <c r="C200">
+        <v>6</v>
+      </c>
+      <c r="D200">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201">
+        <v>13</v>
+      </c>
+      <c r="C201">
+        <v>7</v>
+      </c>
+      <c r="D201">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202">
+        <v>13</v>
+      </c>
+      <c r="C202">
+        <v>8</v>
+      </c>
+      <c r="D202">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203">
+        <v>13</v>
+      </c>
+      <c r="C203">
+        <v>9</v>
+      </c>
+      <c r="D203">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204">
+        <v>13</v>
+      </c>
+      <c r="C204">
+        <v>10</v>
+      </c>
+      <c r="D204">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205">
+        <v>13</v>
+      </c>
+      <c r="C205">
+        <v>11</v>
+      </c>
+      <c r="D205">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206">
+        <v>13</v>
+      </c>
+      <c r="C206">
+        <v>12</v>
+      </c>
+      <c r="D206">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207">
+        <v>13</v>
+      </c>
+      <c r="C207">
+        <v>13</v>
+      </c>
+      <c r="D207">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208">
+        <v>13</v>
+      </c>
+      <c r="C208">
+        <v>14</v>
+      </c>
+      <c r="D208">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209">
+        <v>13</v>
+      </c>
+      <c r="C209">
+        <v>15</v>
+      </c>
+      <c r="D209">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210">
+        <v>13</v>
+      </c>
+      <c r="C210">
+        <v>16</v>
+      </c>
+      <c r="D210">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211">
+        <v>13</v>
+      </c>
+      <c r="C211">
+        <v>17</v>
+      </c>
+      <c r="D211">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212">
+        <v>13</v>
+      </c>
+      <c r="C212">
+        <v>18</v>
+      </c>
+      <c r="D212">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213">
+        <v>13</v>
+      </c>
+      <c r="C213">
+        <v>19</v>
+      </c>
+      <c r="D213">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214">
+        <v>13</v>
+      </c>
+      <c r="C214">
+        <v>20</v>
+      </c>
+      <c r="D214">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215">
+        <v>13</v>
+      </c>
+      <c r="C215">
+        <v>21</v>
+      </c>
+      <c r="D215">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216">
+        <v>13</v>
+      </c>
+      <c r="C216">
+        <v>22</v>
+      </c>
+      <c r="D216">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217">
+        <v>13</v>
+      </c>
+      <c r="C217">
+        <v>23</v>
+      </c>
+      <c r="D217">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218">
+        <v>13</v>
+      </c>
+      <c r="C218">
+        <v>24</v>
+      </c>
+      <c r="D218">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219">
+        <v>13</v>
+      </c>
+      <c r="C219">
+        <v>25</v>
+      </c>
+      <c r="D219">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220">
+        <v>13</v>
+      </c>
+      <c r="C220">
+        <v>26</v>
+      </c>
+      <c r="D220">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221">
+        <v>13</v>
+      </c>
+      <c r="C221">
+        <v>27</v>
+      </c>
+      <c r="D221">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222">
+        <v>13</v>
+      </c>
+      <c r="C222">
+        <v>28</v>
+      </c>
+      <c r="D222">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223">
+        <v>13</v>
+      </c>
+      <c r="C223">
+        <v>29</v>
+      </c>
+      <c r="D223">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224">
+        <v>13</v>
+      </c>
+      <c r="C224">
+        <v>30</v>
+      </c>
+      <c r="D224">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225">
+        <v>13</v>
+      </c>
+      <c r="C225">
+        <v>31</v>
+      </c>
+      <c r="D225">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226">
+        <v>13</v>
+      </c>
+      <c r="C226">
+        <v>32</v>
+      </c>
+      <c r="D226">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227">
+        <v>13</v>
+      </c>
+      <c r="C227">
+        <v>33</v>
+      </c>
+      <c r="D227">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228">
+        <v>13</v>
+      </c>
+      <c r="C228">
+        <v>34</v>
+      </c>
+      <c r="D228">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229">
+        <v>13</v>
+      </c>
+      <c r="C229">
+        <v>35</v>
+      </c>
+      <c r="D229">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230">
+        <v>13</v>
+      </c>
+      <c r="C230">
+        <v>36</v>
+      </c>
+      <c r="D230">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231">
+        <v>13</v>
+      </c>
+      <c r="C231">
+        <v>37</v>
+      </c>
+      <c r="D231">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232">
+        <v>13</v>
+      </c>
+      <c r="C232">
+        <v>38</v>
+      </c>
+      <c r="D232">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233">
+        <v>13</v>
+      </c>
+      <c r="C233">
+        <v>39</v>
+      </c>
+      <c r="D233">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234">
+        <v>13</v>
+      </c>
+      <c r="C234">
+        <v>40</v>
+      </c>
+      <c r="D234">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235">
+        <v>13</v>
+      </c>
+      <c r="C235">
+        <v>41</v>
+      </c>
+      <c r="D235">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236">
+        <v>13</v>
+      </c>
+      <c r="C236">
+        <v>42</v>
+      </c>
+      <c r="D236">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237">
+        <v>13</v>
+      </c>
+      <c r="C237">
+        <v>43</v>
+      </c>
+      <c r="D237">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238">
+        <v>13</v>
+      </c>
+      <c r="C238">
+        <v>44</v>
+      </c>
+      <c r="D238">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239">
+        <v>13</v>
+      </c>
+      <c r="C239">
+        <v>45</v>
+      </c>
+      <c r="D239">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240">
+        <v>13</v>
+      </c>
+      <c r="C240">
+        <v>46</v>
+      </c>
+      <c r="D240">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241">
+        <v>13</v>
+      </c>
+      <c r="C241">
+        <v>47</v>
+      </c>
+      <c r="D241">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242">
+        <v>13</v>
+      </c>
+      <c r="C242">
+        <v>48</v>
+      </c>
+      <c r="D242">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243">
+        <v>13</v>
+      </c>
+      <c r="C243">
+        <v>49</v>
+      </c>
+      <c r="D243">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244">
+        <v>13</v>
+      </c>
+      <c r="C244">
+        <v>50</v>
+      </c>
+      <c r="D244">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245">
+        <v>13</v>
+      </c>
+      <c r="C245">
+        <v>51</v>
+      </c>
+      <c r="D245">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246">
+        <v>13</v>
+      </c>
+      <c r="C246">
+        <v>52</v>
+      </c>
+      <c r="D246">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247">
+        <v>13</v>
+      </c>
+      <c r="C247">
+        <v>53</v>
+      </c>
+      <c r="D247">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248">
+        <v>13</v>
+      </c>
+      <c r="C248">
+        <v>54</v>
+      </c>
+      <c r="D248">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249">
+        <v>13</v>
+      </c>
+      <c r="C249">
+        <v>55</v>
+      </c>
+      <c r="D249">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250">
+        <v>13</v>
+      </c>
+      <c r="C250">
+        <v>56</v>
+      </c>
+      <c r="D250">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251">
+        <v>13</v>
+      </c>
+      <c r="C251">
+        <v>57</v>
+      </c>
+      <c r="D251">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252">
+        <v>13</v>
+      </c>
+      <c r="C252">
+        <v>58</v>
+      </c>
+      <c r="D252">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253">
+        <v>13</v>
+      </c>
+      <c r="C253">
+        <v>59</v>
+      </c>
+      <c r="D253">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254">
+        <v>13</v>
+      </c>
+      <c r="C254">
+        <v>60</v>
+      </c>
+      <c r="D254">
+        <v>1.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>